<commit_message>
Final Order customer checkout
</commit_message>
<xml_diff>
--- a/resources/testdata/OrderCustomerBCT.xlsx
+++ b/resources/testdata/OrderCustomerBCT.xlsx
@@ -4,25 +4,33 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="TestForOrderProvisioned" sheetId="9" r:id="rId2"/>
-    <sheet name="approvedOrderFromISP" sheetId="7" r:id="rId3"/>
-    <sheet name="createOrder" sheetId="2" r:id="rId4"/>
-    <sheet name="upsizeOrder" sheetId="3" r:id="rId5"/>
-    <sheet name="downsizeOrder" sheetId="4" r:id="rId6"/>
-    <sheet name="upgradeOrder" sheetId="5" r:id="rId7"/>
-    <sheet name="downgradeOrder" sheetId="6" r:id="rId8"/>
-    <sheet name="cancleFromStableState" sheetId="8" r:id="rId9"/>
+    <sheet name="approvedUpsizeOrderFromISP" sheetId="10" r:id="rId2"/>
+    <sheet name="TestForOrderProvisioned" sheetId="9" r:id="rId3"/>
+    <sheet name="approvedOrderFromISP" sheetId="7" r:id="rId4"/>
+    <sheet name="createOrder" sheetId="2" r:id="rId5"/>
+    <sheet name="upsizeOrder" sheetId="3" r:id="rId6"/>
+    <sheet name="downsizeOrder" sheetId="4" r:id="rId7"/>
+    <sheet name="upgradeOrder" sheetId="5" r:id="rId8"/>
+    <sheet name="downgradeOrder" sheetId="6" r:id="rId9"/>
+    <sheet name="cancleFromStableState" sheetId="8" r:id="rId10"/>
+    <sheet name="TestForOrderUpsized" sheetId="11" r:id="rId11"/>
+    <sheet name="approvedDownsizeOrderFromISP" sheetId="12" r:id="rId12"/>
+    <sheet name="TestForOrderDownsized" sheetId="13" r:id="rId13"/>
+    <sheet name="approvedUpgradeOrderFromISP" sheetId="14" r:id="rId14"/>
+    <sheet name="TestForOrderUpgraded" sheetId="15" r:id="rId15"/>
+    <sheet name="approvedDowngradeOrderFromISP" sheetId="16" r:id="rId16"/>
+    <sheet name="TestForOrderDowngrade" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -66,42 +74,21 @@
     <t>itemDetails</t>
   </si>
   <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Automation Order One</t>
-  </si>
-  <si>
-    <t>{"ItemList":[{"itemName":"Annual Provisionable Item","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"Camera Megapixel","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"5"},{"itemName":"Extended Warranty","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"4"},{"itemName":"External Memory Card","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"2"},{"itemName":"Ram PPU","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"Ram Reserved","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"0"}]}</t>
-  </si>
-  <si>
     <t>provInfoDetails</t>
   </si>
   <si>
-    <t>orderuserbct@ocusbct.com</t>
-  </si>
-  <si>
-    <t>{"ProvInfoLst":[{"provInfoName":"UserName","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"pratap@domain.com"},{"provInfoName":"Email","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"pratap@domain.com"},{"provInfoName":"Confirm  Email","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"pratap@domain.com"},{"provInfoName":"Handset Color","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"Red"},{"provInfoName":"HeadsetLength","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"35cm"},{"provInfoName":"HandsetModelNumber *","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"Ensim35k"},{"provInfoName":"Phone Password","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"Ensim35k"},{"provInfoName":"Confirm  Phone Password","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"Ensim35k"},{"provInfoName":"Handset Integer","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"123456"},{"provInfoName":"Will you recommend","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"123456"},{"provInfoName":"Default Language","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"English (US)"},{"provInfoName":"Handset Domain","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"customerbct.com"},{"provInfoName":"Purchase Order Number","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"123-8978-67897"},{"provInfoName":"Custom Field1 *","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz"}]}</t>
-  </si>
-  <si>
     <t>upsizeOrder</t>
   </si>
   <si>
     <t>Upsize order</t>
   </si>
   <si>
-    <t>{"ItemList":[{"itemName":"Annual Provisionable Item","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"Camera Megapixel","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"8"},{"itemName":"Extended Warranty","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"6"},{"itemName":"External Memory Card","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"3"},{"itemName":"Ram PPU","operation":"False","textbox":"True","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"Ram Reserved","operation":"False","textbox":"False","dropdown":"False","checkbox":"True","value":"0"}]}</t>
-  </si>
-  <si>
     <t>downsizeOrder</t>
   </si>
   <si>
     <t>Downsize an order</t>
   </si>
   <si>
-    <t>{"ItemList":[{"itemName":"Annual Provisionable Item","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"Camera Megapixel","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"4"},{"itemName":"Extended Warranty","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"2"},{"itemName":"External Memory Card","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"1"},{"itemName":"Ram PPU","operation":"False","textbox":"True","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"Ram Reserved","operation":"False","textbox":"False","dropdown":"False","checkbox":"True","value":"0"}]}</t>
-  </si>
-  <si>
     <t>upgradeOrder</t>
   </si>
   <si>
@@ -111,15 +98,6 @@
     <t>upgradeOfferName</t>
   </si>
   <si>
-    <t>Automation Order two</t>
-  </si>
-  <si>
-    <t>{"ItemList":[{"itemName":"Annual Provisionable Item","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"Ram PPU","operation":"True","textbox":"True","dropdown":"False","checkbox":"True","value":"6"},{"itemName":"External Memory Card","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"5"}]}</t>
-  </si>
-  <si>
-    <t>{"ProvInfoLst":[{"provInfoName":"UserName","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"pratap@domain.com"},{"provInfoName":"Email","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"pratap@domain.com"},{"provInfoName":"Confirm  Email","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"pratap@domain.com"},{"provInfoName":"Handset Color","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"Red"},{"provInfoName":"Handset Integer","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"123456"},{"provInfoName":"Will you recommend","operation":"False","textbox":"False","dropdown":"False","checkbox":"True","value":"123456"},{"provInfoName":"Default Language","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"English (US)"},{"provInfoName":"Handset Domain","operation":"False","textbox":"True","dropdown":"False","checkbox":"False","value":"customerbct.com"},{"provInfoName":"Purchase Order Number","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"123-8978-67897"},{"provInfoName":"Custom Field1 *","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz"}]}</t>
-  </si>
-  <si>
     <t>downgradeOrder</t>
   </si>
   <si>
@@ -129,9 +107,6 @@
     <t>downgradeOfferName</t>
   </si>
   <si>
-    <t>{"ProvInfoLst":[{"provInfoName":"UserName","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"pratap@domain.com"},{"provInfoName":"Email","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"pratap@domain.com"},{"provInfoName":"Handset Color","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"Red"},{"provInfoName":"HeadsetLength","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"35cm"},{"provInfoName":"HandsetModelNumber *","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"Ensim35k"},{"provInfoName":"Phone Password","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"Ensim35k"},{"provInfoName":"Handset Integer","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"123456"},{"provInfoName":"Will you recommend","operation":"False","textbox":"False","dropdown":"False","checkbox":"True","value":"123456"},{"provInfoName":"Default Language","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"English (US)"},{"provInfoName":"Handset Domain","operation":"false","textbox":"False","dropdown":"True","checkbox":"False","value":"customerbct.com"},{"provInfoName":"Purchase Order Number","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"123-8978-67897"},{"provInfoName":"Custom Field1 *","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz"}]}</t>
-  </si>
-  <si>
     <t>cancleFromStableState</t>
   </si>
   <si>
@@ -165,16 +140,94 @@
     <t>purchesOrderNo</t>
   </si>
   <si>
-    <t>xyz-abc-sdrf-dfrc</t>
-  </si>
-  <si>
     <t>approvedOrderFromISP</t>
   </si>
   <si>
     <t>approved a order from ISP side</t>
   </si>
   <si>
-    <t>vgty-76yu-jyuhty-jhkuyu-asdf</t>
+    <t>test34@10044.escm.local</t>
+  </si>
+  <si>
+    <t>MyCloud Service</t>
+  </si>
+  <si>
+    <t>{"ItemList":[{"itemName":"Disk Quota1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"User Quota1","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"5"},{"itemName":"Disk Quota PPU1","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"0"},{"itemName":"User Quota PPU1","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"2"},{"itemName":"User Quota2","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"30.0"},{"itemName":"Disk Quota2","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"2"}]}</t>
+  </si>
+  <si>
+    <t>MyCloud Offer</t>
+  </si>
+  <si>
+    <t>{"ProvInfoLst":[{"provInfoName":"Organization Name *","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"My Test ORG"},{"provInfoName":"Domain Name","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"mytestdomain.com"},{"provInfoName":"BooleanType","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"pratap@domain.com"},{"provInfoName":"PrivateDomainName","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"test34.com"},{"provInfoName":"List of values","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"DisplayName1"},{"provInfoName":"Purchase Order Number","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz-abc-fgtd-dcrt-tfdtc-asdef"},{"provInfoName":"Custom Field1 *","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz"}]}</t>
+  </si>
+  <si>
+    <t>xyz-abc-fgtd-dcrt-tfdtc-asdef</t>
+  </si>
+  <si>
+    <t>{"ItemList":[{"itemName":"Disk Quota1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"User Quota1","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"8"},{"itemName":"Disk Quota PPU1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"User Quota PPU1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"7"},{"itemName":"User Quota2","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"40.0"},{"itemName":"Disk Quota2","operation":"False","textbox":"True","dropdown":"False","checkbox":"False","value":"2"}]}</t>
+  </si>
+  <si>
+    <t>approvedUpsizeOrderFromISP</t>
+  </si>
+  <si>
+    <t>approved a upsize order from ISP side</t>
+  </si>
+  <si>
+    <t>TestForOrderUpsized</t>
+  </si>
+  <si>
+    <t>test order upsized</t>
+  </si>
+  <si>
+    <t>{"ItemList":[{"itemName":"Disk Quota1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"User Quota1","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"4"},{"itemName":"Disk Quota PPU1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"0"},{"itemName":"User Quota PPU1","operation":"False","textbox":"False","dropdown":"False","checkbox":"False","value":"7"},{"itemName":"User Quota2","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"30.0"},{"itemName":"Disk Quota2","operation":"False","textbox":"True","dropdown":"False","checkbox":"False","value":"2"}]}</t>
+  </si>
+  <si>
+    <t>approvedDownsizeOrderFromISP</t>
+  </si>
+  <si>
+    <t>App downsize</t>
+  </si>
+  <si>
+    <t>TestForOrderDownsized</t>
+  </si>
+  <si>
+    <t>order Downsized check</t>
+  </si>
+  <si>
+    <t>MyCloud Offer To Upgrade</t>
+  </si>
+  <si>
+    <t>{"ProvInfoLst":[{"provInfoName":"BooleanType","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"pratap@domain.com"},{"provInfoName":"List of values","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"DisplayName2"},{"provInfoName":"Custom Field2","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz2"}]}</t>
+  </si>
+  <si>
+    <t>approvedUpgradeOrderFromISP</t>
+  </si>
+  <si>
+    <t>approve upgrade order</t>
+  </si>
+  <si>
+    <t>Test for order upgrade</t>
+  </si>
+  <si>
+    <t>TestForOrderDowngrade</t>
+  </si>
+  <si>
+    <t>MyCloud Offer To Downgrade</t>
+  </si>
+  <si>
+    <t>{"ProvInfoLst":[{"provInfoName":"BooleanType","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"pratap@domain.com"},{"provInfoName":"List of values","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"DisplayName3"},{"provInfoName":"Custom Field3","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz3"}]}</t>
+  </si>
+  <si>
+    <t>approvedDowngradeOrderFromISP</t>
+  </si>
+  <si>
+    <t>downgrade approve order</t>
+  </si>
+  <si>
+    <t>TestForOrderUpgraded</t>
+  </si>
+  <si>
+    <t>Test order downgrade</t>
   </si>
 </sst>
 </file>
@@ -233,11 +286,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -543,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,10 +635,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -590,10 +646,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -601,10 +657,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -612,10 +668,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -623,10 +679,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -634,10 +690,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -645,12 +701,100 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -660,7 +804,415 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="orderuserbct@ocusbct.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="orderuserbct@ocusbct.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="orderuserbct@ocusbct.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="orderuserbct@ocusbct.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="orderuserbct@ocusbct.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="orderuserbct@ocusbct.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="orderuserbct@ocusbct.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="orderuserbct@ocusbct.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -683,18 +1235,18 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -705,12 +1257,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,18 +1280,18 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -750,12 +1302,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,30 +1340,30 @@
         <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
+        <v>39</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -822,12 +1374,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,16 +1406,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -874,7 +1426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -906,16 +1458,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -926,12 +1478,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,33 +1506,33 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -991,12 +1543,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,91 +1572,33 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for ms sql
</commit_message>
<xml_diff>
--- a/resources/testdata/OrderCustomerBCT.xlsx
+++ b/resources/testdata/OrderCustomerBCT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="14" activeTab="16"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -212,9 +212,6 @@
     <t>Test order downgrade</t>
   </si>
   <si>
-    <t>orderuser1@10013.escm.local</t>
-  </si>
-  <si>
     <t>My Cloud</t>
   </si>
   <si>
@@ -228,6 +225,9 @@
   </si>
   <si>
     <t>{"ProvInfoLst":[{"provInfoName":"Organization Name *","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"My Test ORG"},{"provInfoName":"Domain Name","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"mytestdomain.com"},{"provInfoName":"BooleanType","operation":"True","textbox":"False","dropdown":"False","checkbox":"True","value":"pratap@domain.com"},{"provInfoName":"PrivateDomainName","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"test34.com"},{"provInfoName":"List of values","operation":"True","textbox":"False","dropdown":"True","checkbox":"False","value":"DisplayName1"},{"provInfoName":"Purchase Order Number","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"abcd-efgh-cdfc-asdf-fgtyd"},{"provInfoName":"Custom Field2 *","operation":"True","textbox":"True","dropdown":"False","checkbox":"False","value":"xyz"}]}</t>
+  </si>
+  <si>
+    <t>orderuser1@10004.escm.local</t>
   </si>
 </sst>
 </file>
@@ -808,7 +808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -839,7 +839,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -896,7 +896,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -941,7 +941,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +984,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1029,7 +1029,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1074,7 +1074,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1119,7 +1119,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1164,7 +1164,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1204,7 +1204,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1249,7 +1249,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1294,7 +1294,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1310,12 +1310,12 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
@@ -1348,13 +1348,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>39</v>
@@ -1366,7 +1366,7 @@
         <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1486,7 +1486,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1535,7 +1535,7 @@
         <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1551,7 +1551,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1586,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1601,7 +1601,7 @@
         <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>